<commit_message>
working on fish prices.
</commit_message>
<xml_diff>
--- a/intermediateTables/PreCATFishesOriginV2.xlsx
+++ b/intermediateTables/PreCATFishesOriginV2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DocsHDD\FGame\中鱼\StatDemo\intermediateTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA5E245-6B44-43E0-B7B4-87D5234EF325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E40331B-A386-49B5-A7A1-B5797851128B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="816" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="34740" windowHeight="20985" tabRatio="816" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="鱼种设计表" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2586" uniqueCount="762">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2643" uniqueCount="775">
   <si>
     <t>Species</t>
   </si>
@@ -1162,6 +1162,12 @@
   </si>
   <si>
     <t>global_temp_tolerence_width</t>
+  </si>
+  <si>
+    <t>舒适温度 min (℃)</t>
+  </si>
+  <si>
+    <t>舒适温度 max (℃)</t>
   </si>
   <si>
     <t>后缀</t>
@@ -3421,6 +3427,41 @@
   </si>
   <si>
     <t>26 ndep.nv.gov</t>
+  </si>
+  <si>
+    <t>o4-mini-h</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>o4mh-deep</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 (估计)</t>
+  </si>
+  <si>
+    <t>21 (估计)</t>
+  </si>
+  <si>
+    <t>16 (推测)</t>
+  </si>
+  <si>
+    <t>27 (推测)</t>
+  </si>
+  <si>
+    <t>30 (估计)</t>
+  </si>
+  <si>
+    <t>15 (估计)</t>
+  </si>
+  <si>
+    <t>26 (估计)</t>
+  </si>
+  <si>
+    <t>12 (估计)</t>
+  </si>
+  <si>
+    <t>33 (估计)</t>
   </si>
 </sst>
 </file>
@@ -4293,10 +4334,10 @@
   <dimension ref="A1:CB24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="AM2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4391,16 +4432,16 @@
         <v>21</v>
       </c>
       <c r="W1" s="61" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="X1" s="61" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="Y1" s="61" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="Z1" s="61" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="AA1" s="10" t="s">
         <v>22</v>
@@ -4421,25 +4462,25 @@
         <v>27</v>
       </c>
       <c r="AG1" s="55" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="AH1" s="55" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="AI1" s="55" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="AJ1" s="55" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="AK1" s="55" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="AL1" s="55" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="AM1" s="55" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="AN1" s="6" t="s">
         <v>28</v>
@@ -4571,7 +4612,7 @@
         <v>Alewife</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>88</v>
@@ -4583,13 +4624,13 @@
         <v>1</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="G2" s="13">
         <v>200</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="I2" s="13">
         <v>1</v>
@@ -4819,7 +4860,7 @@
         <v>Common_Shiner</v>
       </c>
       <c r="B3" s="49" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>88</v>
@@ -4831,13 +4872,13 @@
         <v>1.2</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="G3" s="13">
         <v>240</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="I3" s="13">
         <v>1</v>
@@ -5083,7 +5124,7 @@
         <v>340</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="I4" s="13">
         <v>1</v>
@@ -5313,13 +5354,13 @@
         <v>Pumpkinseed_Sunfish</v>
       </c>
       <c r="B5" s="78" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="C5" s="79" t="s">
         <v>70</v>
       </c>
       <c r="D5" s="79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" s="79">
         <v>1.5</v>
@@ -5329,7 +5370,7 @@
         <v>300</v>
       </c>
       <c r="H5" s="79" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="I5" s="79">
         <v>1</v>
@@ -5370,7 +5411,7 @@
       </c>
       <c r="T5" s="81">
         <f>IF(C5="保底",0,VLOOKUP($D5,'等阶-水温阈值'!$A$1:$B$6,2,FALSE))</f>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="U5" s="82" t="s">
         <v>71</v>
@@ -5559,7 +5600,7 @@
         <v>Bluegill_Sunfish</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>70</v>
@@ -5575,7 +5616,7 @@
         <v>400</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="I6" s="13">
         <v>1</v>
@@ -5805,7 +5846,7 @@
         <v>Redear_Sunfish</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>70</v>
@@ -5821,7 +5862,7 @@
         <v>460</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="I7" s="13">
         <v>1</v>
@@ -6051,7 +6092,7 @@
         <v>Yaqui_Sucker</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>70</v>
@@ -6067,7 +6108,7 @@
         <v>800</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="I8" s="13">
         <v>1</v>
@@ -6297,7 +6338,7 @@
         <v>Buffalofish</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>70</v>
@@ -6313,7 +6354,7 @@
         <v>800</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="I9" s="13">
         <v>1</v>
@@ -6543,7 +6584,7 @@
         <v>Bigmouth_Buffalo</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>70</v>
@@ -6559,7 +6600,7 @@
         <v>1000</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="I10" s="13">
         <v>1</v>
@@ -6789,7 +6830,7 @@
         <v>Tench</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>70</v>
@@ -6805,7 +6846,7 @@
         <v>1600</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="I11" s="13">
         <v>1</v>
@@ -7035,7 +7076,7 @@
         <v>Channel_Catfish</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>70</v>
@@ -7051,7 +7092,7 @@
         <v>1800</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="I12" s="13">
         <v>1</v>
@@ -7281,7 +7322,7 @@
         <v>Common_Shiner</v>
       </c>
       <c r="B13" s="88" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="C13" s="89" t="s">
         <v>88</v>
@@ -7297,7 +7338,7 @@
         <v>200</v>
       </c>
       <c r="H13" s="89" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="I13" s="89">
         <v>2</v>
@@ -7527,7 +7568,7 @@
         <v>Bluegill_Sunfish</v>
       </c>
       <c r="B14" s="78" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="C14" s="79" t="s">
         <v>88</v>
@@ -7773,7 +7814,7 @@
         <v>Redear_Sunfish</v>
       </c>
       <c r="B15" s="78" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="C15" s="79" t="s">
         <v>88</v>
@@ -8019,7 +8060,7 @@
         <v>American_Shad</v>
       </c>
       <c r="B16" s="78" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="C16" s="79" t="s">
         <v>88</v>
@@ -8265,7 +8306,7 @@
         <v>Rock_Bass</v>
       </c>
       <c r="B17" s="78" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="C17" s="79" t="s">
         <v>88</v>
@@ -8511,7 +8552,7 @@
         <v>Bowfin</v>
       </c>
       <c r="B18" s="78" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="C18" s="79" t="s">
         <v>70</v>
@@ -8757,7 +8798,7 @@
         <v>Yellow_Perch</v>
       </c>
       <c r="B19" s="84" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="C19" s="81" t="s">
         <v>70</v>
@@ -8773,7 +8814,7 @@
         <v>900</v>
       </c>
       <c r="H19" s="79" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="I19" s="79">
         <v>2</v>
@@ -9003,7 +9044,7 @@
         <v>Redfin_Pickerel</v>
       </c>
       <c r="B20" s="78" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="C20" s="79" t="s">
         <v>70</v>
@@ -9019,7 +9060,7 @@
         <v>1000</v>
       </c>
       <c r="H20" s="79" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="I20" s="79">
         <v>2</v>
@@ -9249,7 +9290,7 @@
         <v>Spotted_Bass</v>
       </c>
       <c r="B21" s="78" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="C21" s="79" t="s">
         <v>70</v>
@@ -9265,7 +9306,7 @@
         <v>2000</v>
       </c>
       <c r="H21" s="79" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="I21" s="79">
         <v>2</v>
@@ -9495,7 +9536,7 @@
         <v>Largemouth_Bass</v>
       </c>
       <c r="B22" s="78" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="C22" s="79" t="s">
         <v>70</v>
@@ -9511,7 +9552,7 @@
         <v>3200</v>
       </c>
       <c r="H22" s="79" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="I22" s="79">
         <v>2</v>
@@ -9741,7 +9782,7 @@
         <v>American_Eel</v>
       </c>
       <c r="B23" s="78" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="C23" s="79" t="s">
         <v>70</v>
@@ -9753,13 +9794,13 @@
         <v>5</v>
       </c>
       <c r="F23" s="79" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="G23" s="79">
         <v>3200</v>
       </c>
       <c r="H23" s="79" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="I23" s="79">
         <v>2</v>
@@ -9989,7 +10030,7 @@
         <v>Walleye</v>
       </c>
       <c r="B24" s="78" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="C24" s="79" t="s">
         <v>70</v>
@@ -10005,7 +10046,7 @@
         <v>3800</v>
       </c>
       <c r="H24" s="79" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="I24" s="79">
         <v>2</v>
@@ -16842,7 +16883,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -17434,13 +17475,13 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="69" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="B30" s="69" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="C30" s="69" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="D30" s="69" t="s">
         <v>148</v>
@@ -17454,13 +17495,13 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="69" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="B31" s="69" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="C31" s="69" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="D31" s="69" t="s">
         <v>73</v>
@@ -17578,17 +17619,17 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="54" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="B37" s="54" t="str">
         <f t="shared" si="0"/>
         <v>Yaqui_Sucker</v>
       </c>
       <c r="C37" s="66" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="D37" s="49" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="E37" s="54">
         <v>5.2500000000000003E-3</v>
@@ -17599,17 +17640,17 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="54" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="B38" s="54" t="str">
         <f t="shared" si="0"/>
         <v>Bigmouth_Buffalo</v>
       </c>
       <c r="C38" s="66" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="D38" s="49" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="E38" s="54">
         <v>1.6199999999999999E-2</v>
@@ -17620,17 +17661,17 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="54" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="B39" s="54" t="str">
         <f t="shared" si="0"/>
         <v>American_Shad</v>
       </c>
       <c r="C39" s="66" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="D39" s="51" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="E39" s="54">
         <v>6.4599999999999996E-3</v>
@@ -17641,17 +17682,17 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="54" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="B40" s="54" t="str">
         <f t="shared" si="0"/>
         <v>Redfin_Pickerel</v>
       </c>
       <c r="C40" s="66" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="D40" s="49" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="E40" s="54">
         <v>4.79E-3</v>
@@ -19692,7 +19733,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="C2:D24"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27" customHeight="1"/>
@@ -19706,7 +19747,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="27" customHeight="1">
       <c r="A1" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>1</v>
@@ -19717,7 +19758,9 @@
       <c r="D1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="18"/>
+      <c r="E1" s="18" t="s">
+        <v>764</v>
+      </c>
       <c r="F1" s="18" t="s">
         <v>0</v>
       </c>
@@ -19725,16 +19768,26 @@
         <v>1</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>727</v>
-      </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
+        <v>729</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>765</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>370</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>371</v>
+      </c>
       <c r="O1" s="18"/>
       <c r="P1" s="18"/>
       <c r="Q1" s="18"/>
@@ -19762,15 +19815,23 @@
         <v>144</v>
       </c>
       <c r="H2" s="86" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="I2" s="86" t="s">
-        <v>729</v>
-      </c>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
+        <v>731</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="M2" s="19">
+        <v>11</v>
+      </c>
+      <c r="N2" s="19">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" spans="1:17" ht="27" customHeight="1">
       <c r="A3" t="str">
@@ -19789,21 +19850,29 @@
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="19" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="G3" s="19" t="s">
         <v>148</v>
       </c>
       <c r="H3" s="86" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="I3" s="86" t="s">
+        <v>734</v>
+      </c>
+      <c r="K3" s="19" t="s">
         <v>732</v>
       </c>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
+      <c r="L3" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="M3" s="19">
+        <v>17</v>
+      </c>
+      <c r="N3" s="19">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:17" ht="27" customHeight="1">
       <c r="A4" t="str">
@@ -19828,15 +19897,23 @@
         <v>75</v>
       </c>
       <c r="H4" s="86" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="I4" s="86" t="s">
-        <v>734</v>
-      </c>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
+        <v>736</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" s="19">
+        <v>16</v>
+      </c>
+      <c r="N4" s="19">
+        <v>28</v>
+      </c>
     </row>
     <row r="5" spans="1:17" ht="27" customHeight="1">
       <c r="A5" t="str">
@@ -19861,15 +19938,23 @@
         <v>84</v>
       </c>
       <c r="H5" s="86" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="I5" s="86" t="s">
-        <v>734</v>
-      </c>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
+        <v>736</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="L5" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="M5" s="19">
+        <v>21</v>
+      </c>
+      <c r="N5" s="19">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:17" ht="27" customHeight="1">
       <c r="A6" t="str">
@@ -19894,15 +19979,23 @@
         <v>89</v>
       </c>
       <c r="H6" s="86" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="I6" s="86" t="s">
-        <v>736</v>
-      </c>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
+        <v>738</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="M6" s="19">
+        <v>18</v>
+      </c>
+      <c r="N6" s="19">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:17" ht="27" customHeight="1">
       <c r="A7" t="str">
@@ -19927,15 +20020,23 @@
         <v>87</v>
       </c>
       <c r="H7" s="86" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="I7" s="86" t="s">
-        <v>734</v>
-      </c>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
+        <v>736</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="L7" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="M7" s="19">
+        <v>21</v>
+      </c>
+      <c r="N7" s="19">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:17" ht="27" customHeight="1">
       <c r="A8" t="str">
@@ -19947,28 +20048,36 @@
         <v>白亚口鱼</v>
       </c>
       <c r="C8" s="19">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D8" s="19">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="19" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>739</v>
-      </c>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
+        <v>741</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>717</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>683</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>766</v>
+      </c>
+      <c r="N8" s="19" t="s">
+        <v>767</v>
+      </c>
     </row>
     <row r="9" spans="1:17" ht="27" customHeight="1">
       <c r="A9" t="str">
@@ -19980,10 +20089,10 @@
         <v>水牛鱼</v>
       </c>
       <c r="C9" s="19">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="19">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="19" t="s">
@@ -19993,15 +20102,23 @@
         <v>85</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>739</v>
-      </c>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
+        <v>741</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="L9" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="M9" s="19" t="s">
+        <v>768</v>
+      </c>
+      <c r="N9" s="19" t="s">
+        <v>769</v>
+      </c>
     </row>
     <row r="10" spans="1:17" ht="27" customHeight="1">
       <c r="A10" t="str">
@@ -20013,28 +20130,36 @@
         <v>大口牛胭脂鱼</v>
       </c>
       <c r="C10" s="19">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D10" s="19">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E10" s="19"/>
       <c r="F10" s="19" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>739</v>
-      </c>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
+        <v>741</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>718</v>
+      </c>
+      <c r="L10" s="19" t="s">
+        <v>571</v>
+      </c>
+      <c r="M10" s="19">
+        <v>16</v>
+      </c>
+      <c r="N10" s="19">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:17" ht="27" customHeight="1">
       <c r="A11" t="str">
@@ -20046,10 +20171,10 @@
         <v>丁鱥</v>
       </c>
       <c r="C11" s="19">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D11" s="19">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="19" t="s">
@@ -20059,15 +20184,23 @@
         <v>69</v>
       </c>
       <c r="H11" s="86" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="I11" s="86" t="s">
-        <v>742</v>
-      </c>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
+        <v>744</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="L11" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11" s="19">
+        <v>4</v>
+      </c>
+      <c r="N11" s="19">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:17" ht="27" customHeight="1">
       <c r="A12" t="str">
@@ -20092,15 +20225,23 @@
         <v>82</v>
       </c>
       <c r="H12" s="86" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="I12" s="86" t="s">
-        <v>744</v>
-      </c>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
+        <v>746</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="L12" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="M12" s="19">
+        <v>24</v>
+      </c>
+      <c r="N12" s="19" t="s">
+        <v>770</v>
+      </c>
     </row>
     <row r="13" spans="1:17" ht="27" customHeight="1">
       <c r="A13" t="str">
@@ -20112,28 +20253,36 @@
         <v>美鳊</v>
       </c>
       <c r="C13" s="19">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D13" s="19">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E13" s="19"/>
       <c r="F13" s="19" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="H13" s="86" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="I13" s="86" t="s">
+        <v>749</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>719</v>
+      </c>
+      <c r="L13" s="19" t="s">
         <v>747</v>
       </c>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
+      <c r="M13" s="19">
+        <v>12</v>
+      </c>
+      <c r="N13" s="19">
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="1:17" ht="27" customHeight="1">
       <c r="A14" t="str">
@@ -20148,7 +20297,7 @@
         <v>18</v>
       </c>
       <c r="D14" s="19">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E14" s="19"/>
       <c r="F14" s="19" t="s">
@@ -20158,15 +20307,23 @@
         <v>97</v>
       </c>
       <c r="H14" s="86" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="I14" s="86" t="s">
-        <v>749</v>
-      </c>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
+        <v>751</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="L14" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="M14" s="19" t="s">
+        <v>771</v>
+      </c>
+      <c r="N14" s="19" t="s">
+        <v>772</v>
+      </c>
     </row>
     <row r="15" spans="1:17" ht="27" customHeight="1">
       <c r="A15" t="str">
@@ -20178,10 +20335,10 @@
         <v>小冠太阳鱼</v>
       </c>
       <c r="C15">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F15" s="19" t="s">
         <v>149</v>
@@ -20190,15 +20347,23 @@
         <v>94</v>
       </c>
       <c r="H15" s="86" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="I15" s="86" t="s">
-        <v>751</v>
-      </c>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
+        <v>753</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="L15" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="M15" s="19" t="s">
+        <v>773</v>
+      </c>
+      <c r="N15" s="19" t="s">
+        <v>772</v>
+      </c>
     </row>
     <row r="16" spans="1:17" ht="27" customHeight="1">
       <c r="A16" t="str">
@@ -20210,10 +20375,10 @@
         <v>美洲西鲱</v>
       </c>
       <c r="C16">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F16" s="19" t="s">
         <v>176</v>
@@ -20222,15 +20387,23 @@
         <v>96</v>
       </c>
       <c r="H16" s="86" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="I16" s="86" t="s">
-        <v>753</v>
-      </c>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
+        <v>755</v>
+      </c>
+      <c r="K16" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="L16" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="M16" s="19">
+        <v>17</v>
+      </c>
+      <c r="N16" s="19">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="1:14" ht="27" customHeight="1">
       <c r="A17" t="str">
@@ -20242,27 +20415,35 @@
         <v>岩钝鲈</v>
       </c>
       <c r="C17">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D17">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>754</v>
-      </c>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
+        <v>756</v>
+      </c>
+      <c r="K17" s="19" t="s">
+        <v>720</v>
+      </c>
+      <c r="L17" s="19" t="s">
+        <v>554</v>
+      </c>
+      <c r="M17" s="19">
+        <v>4</v>
+      </c>
+      <c r="N17" s="19">
+        <v>18</v>
+      </c>
     </row>
     <row r="18" spans="1:14" ht="27" customHeight="1">
       <c r="A18" t="str">
@@ -20286,15 +20467,23 @@
         <v>135</v>
       </c>
       <c r="H18" s="86" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="I18" s="86" t="s">
-        <v>736</v>
-      </c>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
+        <v>738</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>323</v>
+      </c>
+      <c r="L18" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="M18" s="19">
+        <v>15</v>
+      </c>
+      <c r="N18" s="19">
+        <v>23</v>
+      </c>
     </row>
     <row r="19" spans="1:14" ht="27" customHeight="1">
       <c r="A19" t="str">
@@ -20306,10 +20495,10 @@
         <v>黄鲈</v>
       </c>
       <c r="C19">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D19">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F19" s="19" t="s">
         <v>168</v>
@@ -20318,15 +20507,23 @@
         <v>81</v>
       </c>
       <c r="H19" s="86" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="I19" s="86" t="s">
-        <v>757</v>
-      </c>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
+        <v>759</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="L19" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="M19" s="19" t="s">
+        <v>767</v>
+      </c>
+      <c r="N19" s="19" t="s">
+        <v>774</v>
+      </c>
     </row>
     <row r="20" spans="1:14" ht="27" customHeight="1">
       <c r="A20" t="str">
@@ -20338,10 +20535,10 @@
         <v>红鳍狗鱼</v>
       </c>
       <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
         <v>18</v>
-      </c>
-      <c r="D20">
-        <v>28</v>
       </c>
       <c r="F20" s="19" t="s">
         <v>329</v>
@@ -20350,15 +20547,23 @@
         <v>126</v>
       </c>
       <c r="H20" s="86" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="I20" s="86" t="s">
-        <v>759</v>
-      </c>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
+        <v>761</v>
+      </c>
+      <c r="K20" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="L20" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="M20" s="19">
+        <v>4</v>
+      </c>
+      <c r="N20" s="19">
+        <v>25</v>
+      </c>
     </row>
     <row r="21" spans="1:14" ht="27" customHeight="1">
       <c r="A21" t="str">
@@ -20370,10 +20575,10 @@
         <v>斑点黑鲈</v>
       </c>
       <c r="C21">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D21">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F21" s="19" t="s">
         <v>125</v>
@@ -20382,15 +20587,23 @@
         <v>92</v>
       </c>
       <c r="H21" s="86" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="I21" s="86" t="s">
-        <v>761</v>
-      </c>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
+        <v>763</v>
+      </c>
+      <c r="K21" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="L21" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="M21" s="19">
+        <v>20</v>
+      </c>
+      <c r="N21" s="19">
+        <v>24</v>
+      </c>
     </row>
     <row r="22" spans="1:14" ht="27" customHeight="1">
       <c r="A22" t="str">
@@ -20402,10 +20615,10 @@
         <v>大口黑鲈</v>
       </c>
       <c r="C22">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D22">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
@@ -20425,10 +20638,10 @@
         <v>美洲鳗鲡</v>
       </c>
       <c r="C23">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D23">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
@@ -20448,10 +20661,10 @@
         <v>玻璃梭鲈</v>
       </c>
       <c r="C24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D24">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -20513,13 +20726,13 @@
         <v>7</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -20530,7 +20743,7 @@
         <v>165</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="D2" s="12">
         <v>1000</v>
@@ -20544,7 +20757,7 @@
         <v>158</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="D3" s="12">
         <v>1000</v>
@@ -20558,7 +20771,7 @@
         <v>159</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D4" s="12">
         <v>500</v>
@@ -20572,7 +20785,7 @@
         <v>160</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="D5" s="12">
         <v>250</v>
@@ -20586,7 +20799,7 @@
         <v>161</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="D6" s="12">
         <v>100</v>
@@ -20621,34 +20834,34 @@
         <v>178</v>
       </c>
       <c r="B1" s="56" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C1" s="56" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D1" s="56" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="E1" s="56" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="F1" s="56" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="G1" s="56" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="H1" s="56" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="I1" s="56" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="J1" s="56" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="K1" s="56" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -20656,10 +20869,10 @@
         <v>101020001</v>
       </c>
       <c r="B2" s="57" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C2" s="57" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D2" s="57" t="s">
         <v>143</v>
@@ -20668,13 +20881,13 @@
         <v>87</v>
       </c>
       <c r="F2" s="57" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="G2" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H2" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I2" s="58">
         <v>1.5</v>
@@ -20683,7 +20896,7 @@
         <v>0</v>
       </c>
       <c r="K2" s="57" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -20691,10 +20904,10 @@
         <v>101020002</v>
       </c>
       <c r="B3" s="57" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="D3" s="57" t="s">
         <v>317</v>
@@ -20703,13 +20916,13 @@
         <v>85</v>
       </c>
       <c r="F3" s="57" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="G3" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H3" s="57" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="I3" s="58">
         <v>1.8</v>
@@ -20718,7 +20931,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="57" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -20726,10 +20939,10 @@
         <v>101020003</v>
       </c>
       <c r="B4" s="57" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="D4" s="57" t="s">
         <v>149</v>
@@ -20738,13 +20951,13 @@
         <v>94</v>
       </c>
       <c r="F4" s="57" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="G4" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H4" s="57" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="I4" s="58">
         <v>1.2</v>
@@ -20753,7 +20966,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="57" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -20761,10 +20974,10 @@
         <v>101020004</v>
       </c>
       <c r="B5" s="57" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="C5" s="57" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D5" s="57" t="s">
         <v>139</v>
@@ -20773,13 +20986,13 @@
         <v>96</v>
       </c>
       <c r="F5" s="57" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="G5" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H5" s="57" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="I5" s="58">
         <v>2</v>
@@ -20788,7 +21001,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="57" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -20796,10 +21009,10 @@
         <v>101020005</v>
       </c>
       <c r="B6" s="57" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="C6" s="57" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="D6" s="57" t="s">
         <v>138</v>
@@ -20808,13 +21021,13 @@
         <v>82</v>
       </c>
       <c r="F6" s="57" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="G6" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H6" s="57" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="I6" s="58">
         <v>2.8</v>
@@ -20823,7 +21036,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="57" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -20831,10 +21044,10 @@
         <v>101020006</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="C7" s="57" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="D7" s="57" t="s">
         <v>112</v>
@@ -20843,13 +21056,13 @@
         <v>93</v>
       </c>
       <c r="F7" s="57" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="G7" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H7" s="57" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="I7" s="58">
         <v>2.5</v>
@@ -20858,7 +21071,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="57" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -20866,10 +21079,10 @@
         <v>101020007</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="C8" s="57" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="D8" s="57" t="s">
         <v>145</v>
@@ -20878,13 +21091,13 @@
         <v>144</v>
       </c>
       <c r="F8" s="57" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="G8" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H8" s="57" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="I8" s="58">
         <v>2.2000000000000002</v>
@@ -20893,7 +21106,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="57" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -20901,10 +21114,10 @@
         <v>101020008</v>
       </c>
       <c r="B9" s="57" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C9" s="57" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="D9" s="57" t="s">
         <v>110</v>
@@ -20913,13 +21126,13 @@
         <v>91</v>
       </c>
       <c r="F9" s="57" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="G9" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H9" s="57" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="I9" s="58">
         <v>2.4</v>
@@ -20928,7 +21141,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="57" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -20936,25 +21149,25 @@
         <v>101020009</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C10" s="57" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D10" s="57" t="s">
         <v>152</v>
       </c>
       <c r="E10" s="57" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="F10" s="57" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="G10" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H10" s="57" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="I10" s="58">
         <v>1.8</v>
@@ -20963,7 +21176,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="57" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -20971,10 +21184,10 @@
         <v>101020010</v>
       </c>
       <c r="B11" s="57" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C11" s="57" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D11" s="57" t="s">
         <v>320</v>
@@ -20983,13 +21196,13 @@
         <v>321</v>
       </c>
       <c r="F11" s="57" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="G11" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H11" s="57" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="I11" s="58">
         <v>2.5</v>
@@ -20998,7 +21211,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="57" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -21006,10 +21219,10 @@
         <v>101020011</v>
       </c>
       <c r="B12" s="57" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C12" s="57" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="D12" s="57" t="s">
         <v>132</v>
@@ -21018,13 +21231,13 @@
         <v>69</v>
       </c>
       <c r="F12" s="57" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="G12" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H12" s="57" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="I12" s="58">
         <v>1.5</v>
@@ -21033,7 +21246,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="57" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -21041,10 +21254,10 @@
         <v>101020012</v>
       </c>
       <c r="B13" s="57" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="C13" s="57" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="D13" s="57" t="s">
         <v>141</v>
@@ -21053,13 +21266,13 @@
         <v>140</v>
       </c>
       <c r="F13" s="57" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="G13" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H13" s="57" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="I13" s="58">
         <v>1.6</v>
@@ -21068,7 +21281,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="57" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -21076,10 +21289,10 @@
         <v>101020013</v>
       </c>
       <c r="B14" s="57" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C14" s="57" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D14" s="57" t="s">
         <v>121</v>
@@ -21088,13 +21301,13 @@
         <v>81</v>
       </c>
       <c r="F14" s="57" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="G14" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H14" s="57" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="I14" s="58">
         <v>2</v>
@@ -21103,7 +21316,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="57" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -21111,10 +21324,10 @@
         <v>101020014</v>
       </c>
       <c r="B15" s="57" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="C15" s="57" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D15" s="57" t="s">
         <v>136</v>
@@ -21123,13 +21336,13 @@
         <v>135</v>
       </c>
       <c r="F15" s="57" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="G15" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H15" s="57" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="I15" s="58">
         <v>2</v>
@@ -21138,7 +21351,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="57" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -21146,10 +21359,10 @@
         <v>101020015</v>
       </c>
       <c r="B16" s="57" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="C16" s="57" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D16" s="57" t="s">
         <v>118</v>
@@ -21158,13 +21371,13 @@
         <v>117</v>
       </c>
       <c r="F16" s="57" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="G16" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H16" s="57" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="I16" s="58">
         <v>1.6</v>
@@ -21173,7 +21386,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="57" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -21181,10 +21394,10 @@
         <v>101020016</v>
       </c>
       <c r="B17" s="57" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C17" s="57" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D17" s="57" t="s">
         <v>137</v>
@@ -21193,13 +21406,13 @@
         <v>97</v>
       </c>
       <c r="F17" s="57" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="G17" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H17" s="57" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="I17" s="58">
         <v>1.7</v>
@@ -21208,7 +21421,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="57" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -21216,10 +21429,10 @@
         <v>101020017</v>
       </c>
       <c r="B18" s="57" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C18" s="57" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D18" s="57" t="s">
         <v>129</v>
@@ -21228,13 +21441,13 @@
         <v>128</v>
       </c>
       <c r="F18" s="57" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="G18" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H18" s="57" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="I18" s="58">
         <v>2.1</v>
@@ -21243,7 +21456,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="57" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -21251,10 +21464,10 @@
         <v>101020018</v>
       </c>
       <c r="B19" s="57" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C19" s="57" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D19" s="57" t="s">
         <v>124</v>
@@ -21263,13 +21476,13 @@
         <v>95</v>
       </c>
       <c r="F19" s="57" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="G19" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H19" s="57" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="I19" s="58">
         <v>1.6</v>
@@ -21278,7 +21491,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="57" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -21286,10 +21499,10 @@
         <v>101020019</v>
       </c>
       <c r="B20" s="57" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C20" s="57" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D20" s="57" t="s">
         <v>146</v>
@@ -21298,13 +21511,13 @@
         <v>84</v>
       </c>
       <c r="F20" s="57" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="G20" s="57" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="H20" s="57" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="I20" s="58">
         <v>1.5</v>
@@ -21313,7 +21526,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="57" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -21321,10 +21534,10 @@
         <v>101020020</v>
       </c>
       <c r="B21" s="57" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="C21" s="57" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D21" s="57" t="s">
         <v>147</v>
@@ -21333,13 +21546,13 @@
         <v>75</v>
       </c>
       <c r="F21" s="57" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="G21" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H21" s="57" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="I21" s="58">
         <v>1.5</v>
@@ -21348,7 +21561,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="57" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -21356,10 +21569,10 @@
         <v>101020021</v>
       </c>
       <c r="B22" s="57" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="C22" s="57" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D22" s="57" t="s">
         <v>142</v>
@@ -21368,13 +21581,13 @@
         <v>80</v>
       </c>
       <c r="F22" s="57" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="G22" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H22" s="57" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="I22" s="58">
         <v>1.5</v>
@@ -21383,7 +21596,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="57" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -21391,10 +21604,10 @@
         <v>101020022</v>
       </c>
       <c r="B23" s="57" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="C23" s="57" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="D23" s="57" t="s">
         <v>120</v>
@@ -21403,13 +21616,13 @@
         <v>119</v>
       </c>
       <c r="F23" s="57" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="G23" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H23" s="57" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="I23" s="58">
         <v>2.4</v>
@@ -21418,7 +21631,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="57" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -21426,10 +21639,10 @@
         <v>101020023</v>
       </c>
       <c r="B24" s="57" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="C24" s="57" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D24" s="57" t="s">
         <v>134</v>
@@ -21438,13 +21651,13 @@
         <v>133</v>
       </c>
       <c r="F24" s="57" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="G24" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H24" s="57" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="I24" s="58">
         <v>2.2000000000000002</v>
@@ -21453,7 +21666,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="57" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -21461,10 +21674,10 @@
         <v>101020024</v>
       </c>
       <c r="B25" s="57" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="C25" s="57" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D25" s="57" t="s">
         <v>125</v>
@@ -21473,13 +21686,13 @@
         <v>92</v>
       </c>
       <c r="F25" s="57" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="G25" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H25" s="57" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="I25" s="58">
         <v>2.2999999999999998</v>
@@ -21488,7 +21701,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="57" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -21496,10 +21709,10 @@
         <v>101020025</v>
       </c>
       <c r="B26" s="57" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="C26" s="57" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D26" s="57" t="s">
         <v>123</v>
@@ -21508,13 +21721,13 @@
         <v>122</v>
       </c>
       <c r="F26" s="57" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="G26" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H26" s="57" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="I26" s="58">
         <v>2.5</v>
@@ -21523,7 +21736,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="57" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -21531,10 +21744,10 @@
         <v>101020026</v>
       </c>
       <c r="B27" s="57" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="C27" s="57" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D27" s="57" t="s">
         <v>131</v>
@@ -21543,13 +21756,13 @@
         <v>130</v>
       </c>
       <c r="F27" s="57" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="G27" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H27" s="57" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="I27" s="58">
         <v>2.5</v>
@@ -21558,7 +21771,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="57" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -21566,10 +21779,10 @@
         <v>101020027</v>
       </c>
       <c r="B28" s="57" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="C28" s="57" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D28" s="57" t="s">
         <v>328</v>
@@ -21578,13 +21791,13 @@
         <v>89</v>
       </c>
       <c r="F28" s="57" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="G28" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H28" s="57" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="I28" s="58">
         <v>1.5</v>
@@ -21593,7 +21806,7 @@
         <v>0</v>
       </c>
       <c r="K28" s="57" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -21601,10 +21814,10 @@
         <v>101020031</v>
       </c>
       <c r="B29" s="57" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="C29" s="57" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="D29" s="57" t="s">
         <v>127</v>
@@ -21613,13 +21826,13 @@
         <v>126</v>
       </c>
       <c r="F29" s="57" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="G29" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H29" s="57" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="I29" s="58">
         <v>1</v>
@@ -21628,7 +21841,7 @@
         <v>0</v>
       </c>
       <c r="K29" s="57" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -21636,10 +21849,10 @@
         <v>101020032</v>
       </c>
       <c r="B30" s="57" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C30" s="57" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D30" s="57" t="s">
         <v>330</v>
@@ -21648,13 +21861,13 @@
         <v>148</v>
       </c>
       <c r="F30" s="57" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="G30" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H30" s="57" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="I30" s="58">
         <v>1.7</v>
@@ -21663,7 +21876,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="57" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -21671,10 +21884,10 @@
         <v>101020033</v>
       </c>
       <c r="B31" s="57" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="C31" s="57" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D31" s="57" t="s">
         <v>331</v>
@@ -21683,13 +21896,13 @@
         <v>73</v>
       </c>
       <c r="F31" s="57" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="G31" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H31" s="57" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="I31" s="58">
         <v>1.7</v>
@@ -21698,7 +21911,7 @@
         <v>0</v>
       </c>
       <c r="K31" s="57" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -21706,10 +21919,10 @@
         <v>101020034</v>
       </c>
       <c r="B32" s="57" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="C32" s="57" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D32" s="57" t="s">
         <v>333</v>
@@ -21718,13 +21931,13 @@
         <v>150</v>
       </c>
       <c r="F32" s="57" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="G32" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H32" s="57" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="I32" s="58">
         <v>1.8</v>
@@ -21733,7 +21946,7 @@
         <v>0</v>
       </c>
       <c r="K32" s="57" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -21741,25 +21954,25 @@
         <v>101020035</v>
       </c>
       <c r="B33" s="57" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="C33" s="56" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="D33" s="57" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="E33" s="57" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="F33" s="57" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="G33" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H33" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I33" s="58">
         <v>1.5</v>
@@ -21768,7 +21981,7 @@
         <v>0</v>
       </c>
       <c r="K33" s="56" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -21776,10 +21989,10 @@
         <v>101020036</v>
       </c>
       <c r="B34" s="57" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="C34" s="56" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="D34" s="57" t="s">
         <v>116</v>
@@ -21788,13 +22001,13 @@
         <v>115</v>
       </c>
       <c r="F34" s="57" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="G34" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H34" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I34" s="58">
         <v>1.5</v>
@@ -21803,7 +22016,7 @@
         <v>0</v>
       </c>
       <c r="K34" s="56" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -21811,25 +22024,25 @@
         <v>101020037</v>
       </c>
       <c r="B35" s="57" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="C35" s="56" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="D35" s="57" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="E35" s="57" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="F35" s="57" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="G35" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H35" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I35" s="58">
         <v>1.5</v>
@@ -21838,7 +22051,7 @@
         <v>0</v>
       </c>
       <c r="K35" s="56" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -21846,25 +22059,25 @@
         <v>101020038</v>
       </c>
       <c r="B36" s="57" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="C36" s="56" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="D36" s="57" t="s">
         <v>109</v>
       </c>
       <c r="E36" s="57" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="F36" s="57" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="G36" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H36" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I36" s="58">
         <v>1.5</v>
@@ -21873,7 +22086,7 @@
         <v>0</v>
       </c>
       <c r="K36" s="56" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -21881,25 +22094,25 @@
         <v>101020039</v>
       </c>
       <c r="B37" s="57" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="C37" s="56" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="D37" s="57" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="E37" s="57" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="F37" s="57" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="G37" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H37" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I37" s="58">
         <v>1.5</v>
@@ -21908,7 +22121,7 @@
         <v>0</v>
       </c>
       <c r="K37" s="56" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -21916,25 +22129,25 @@
         <v>101020040</v>
       </c>
       <c r="B38" s="57" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="C38" s="56" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="D38" s="57" t="s">
         <v>111</v>
       </c>
       <c r="E38" s="57" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="F38" s="57" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="G38" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H38" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I38" s="58">
         <v>1.5</v>
@@ -21943,7 +22156,7 @@
         <v>0</v>
       </c>
       <c r="K38" s="56" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -21951,25 +22164,25 @@
         <v>101020041</v>
       </c>
       <c r="B39" s="57" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="C39" s="56" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="D39" s="57" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="E39" s="57" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="F39" s="57" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="G39" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H39" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I39" s="58">
         <v>1.5</v>
@@ -21978,7 +22191,7 @@
         <v>0</v>
       </c>
       <c r="K39" s="56" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -21986,25 +22199,25 @@
         <v>101020042</v>
       </c>
       <c r="B40" s="57" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="C40" s="56" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="D40" s="57" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="E40" s="57" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="F40" s="57" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="G40" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H40" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I40" s="58">
         <v>1.5</v>
@@ -22013,7 +22226,7 @@
         <v>0</v>
       </c>
       <c r="K40" s="56" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -22021,10 +22234,10 @@
         <v>101020043</v>
       </c>
       <c r="B41" s="57" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="C41" s="56" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="D41" s="57" t="s">
         <v>104</v>
@@ -22033,13 +22246,13 @@
         <v>103</v>
       </c>
       <c r="F41" s="57" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="G41" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H41" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I41" s="58">
         <v>1.5</v>
@@ -22048,7 +22261,7 @@
         <v>0</v>
       </c>
       <c r="K41" s="56" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -22056,25 +22269,25 @@
         <v>101020044</v>
       </c>
       <c r="B42" s="57" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="C42" s="57" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D42" s="57" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="E42" s="57" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="F42" s="57" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="G42" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H42" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I42" s="58">
         <v>1.5</v>
@@ -22083,7 +22296,7 @@
         <v>0</v>
       </c>
       <c r="K42" s="57" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -22091,25 +22304,25 @@
         <v>101020045</v>
       </c>
       <c r="B43" s="57" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="C43" s="56" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D43" s="57" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="E43" s="57" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="F43" s="57" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="G43" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H43" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I43" s="58">
         <v>1.5</v>
@@ -22118,7 +22331,7 @@
         <v>0</v>
       </c>
       <c r="K43" s="56" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -22126,25 +22339,25 @@
         <v>101020046</v>
       </c>
       <c r="B44" s="57" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="C44" s="56" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="D44" s="57" t="s">
         <v>107</v>
       </c>
       <c r="E44" s="57" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="F44" s="57" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="G44" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H44" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I44" s="58">
         <v>1.5</v>
@@ -22153,7 +22366,7 @@
         <v>0</v>
       </c>
       <c r="K44" s="56" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -22161,25 +22374,25 @@
         <v>101020047</v>
       </c>
       <c r="B45" s="57" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="C45" s="56" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="D45" s="57" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="E45" s="57" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="F45" s="57" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="G45" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H45" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I45" s="58">
         <v>1.5</v>
@@ -22188,7 +22401,7 @@
         <v>0</v>
       </c>
       <c r="K45" s="56" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -22196,25 +22409,25 @@
         <v>101020048</v>
       </c>
       <c r="B46" s="57" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="C46" s="56" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="D46" s="57" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="E46" s="57" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="F46" s="57" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="G46" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H46" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I46" s="58">
         <v>1.5</v>
@@ -22223,7 +22436,7 @@
         <v>0</v>
       </c>
       <c r="K46" s="56" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -22231,25 +22444,25 @@
         <v>101020049</v>
       </c>
       <c r="B47" s="57" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="C47" s="56" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="D47" s="57" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="E47" s="57" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="F47" s="57" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="G47" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H47" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I47" s="58">
         <v>1.5</v>
@@ -22258,7 +22471,7 @@
         <v>0</v>
       </c>
       <c r="K47" s="56" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -22266,25 +22479,25 @@
         <v>101020050</v>
       </c>
       <c r="B48" s="57" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="C48" s="56" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="D48" s="57" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="E48" s="57" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="F48" s="57" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="G48" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H48" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I48" s="58">
         <v>1.5</v>
@@ -22293,7 +22506,7 @@
         <v>0</v>
       </c>
       <c r="K48" s="56" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -22301,25 +22514,25 @@
         <v>101020051</v>
       </c>
       <c r="B49" s="57" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="C49" s="57" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D49" s="57" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="E49" s="57" t="s">
         <v>113</v>
       </c>
       <c r="F49" s="57" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="G49" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H49" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I49" s="58">
         <v>1.5</v>
@@ -22328,7 +22541,7 @@
         <v>0</v>
       </c>
       <c r="K49" s="57" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -22336,25 +22549,25 @@
         <v>101020052</v>
       </c>
       <c r="B50" s="57" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="C50" s="56" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="D50" s="57" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="E50" s="57" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="F50" s="57" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="G50" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H50" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I50" s="58">
         <v>1.5</v>
@@ -22363,7 +22576,7 @@
         <v>0</v>
       </c>
       <c r="K50" s="56" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -22371,25 +22584,25 @@
         <v>101020053</v>
       </c>
       <c r="B51" s="57" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="C51" s="56" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D51" s="57" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="E51" s="57" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="F51" s="57" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="G51" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H51" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I51" s="58">
         <v>1.5</v>
@@ -22398,7 +22611,7 @@
         <v>0</v>
       </c>
       <c r="K51" s="56" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -22406,25 +22619,25 @@
         <v>101020054</v>
       </c>
       <c r="B52" s="57" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="C52" s="56" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D52" s="57" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="E52" s="57" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="F52" s="57" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="G52" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H52" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I52" s="58">
         <v>1.5</v>
@@ -22433,7 +22646,7 @@
         <v>0</v>
       </c>
       <c r="K52" s="56" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -22441,25 +22654,25 @@
         <v>101020055</v>
       </c>
       <c r="B53" s="57" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="C53" s="56" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="D53" s="57" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="E53" s="57" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="F53" s="57" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="G53" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H53" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I53" s="58">
         <v>1.5</v>
@@ -22468,7 +22681,7 @@
         <v>0</v>
       </c>
       <c r="K53" s="56" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -22476,10 +22689,10 @@
         <v>101020056</v>
       </c>
       <c r="B54" s="57" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="C54" s="56" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="D54" s="57" t="s">
         <v>106</v>
@@ -22488,13 +22701,13 @@
         <v>105</v>
       </c>
       <c r="F54" s="57" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="G54" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H54" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I54" s="58">
         <v>1.5</v>
@@ -22503,7 +22716,7 @@
         <v>0</v>
       </c>
       <c r="K54" s="56" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -22511,25 +22724,25 @@
         <v>101020057</v>
       </c>
       <c r="B55" s="57" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="C55" s="56" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="D55" s="57" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="E55" s="57" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="F55" s="57" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="G55" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H55" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I55" s="58">
         <v>1.5</v>
@@ -22538,7 +22751,7 @@
         <v>0</v>
       </c>
       <c r="K55" s="56" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -22546,25 +22759,25 @@
         <v>101020058</v>
       </c>
       <c r="B56" s="57" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="C56" s="56" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="D56" s="57" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="E56" s="57" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="F56" s="57" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="G56" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H56" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I56" s="58">
         <v>1.5</v>
@@ -22573,7 +22786,7 @@
         <v>0</v>
       </c>
       <c r="K56" s="56" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -22581,25 +22794,25 @@
         <v>101020059</v>
       </c>
       <c r="B57" s="57" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="C57" s="56" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="D57" s="57" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="E57" s="57" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="F57" s="57" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="G57" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H57" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I57" s="58">
         <v>1.5</v>
@@ -22608,7 +22821,7 @@
         <v>0</v>
       </c>
       <c r="K57" s="56" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -22616,25 +22829,25 @@
         <v>101020060</v>
       </c>
       <c r="B58" s="57" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="C58" s="57" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D58" s="57" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="E58" s="57" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="F58" s="57" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="G58" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H58" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I58" s="58">
         <v>1.5</v>
@@ -22643,7 +22856,7 @@
         <v>0</v>
       </c>
       <c r="K58" s="57" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -22651,25 +22864,25 @@
         <v>101020061</v>
       </c>
       <c r="B59" s="57" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="C59" s="56" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D59" s="57" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="E59" s="57" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="F59" s="57" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="G59" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H59" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I59" s="58">
         <v>1.5</v>
@@ -22678,7 +22891,7 @@
         <v>0</v>
       </c>
       <c r="K59" s="56" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -22686,25 +22899,25 @@
         <v>101020062</v>
       </c>
       <c r="B60" s="57" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="C60" s="56" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D60" s="57" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="E60" s="57" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="F60" s="57" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="G60" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H60" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I60" s="58">
         <v>1.5</v>
@@ -22713,7 +22926,7 @@
         <v>0</v>
       </c>
       <c r="K60" s="56" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -22721,25 +22934,25 @@
         <v>101020063</v>
       </c>
       <c r="B61" s="57" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="C61" s="56" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D61" s="57" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="E61" s="57" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="F61" s="57" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="G61" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H61" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I61" s="58">
         <v>1.5</v>
@@ -22748,7 +22961,7 @@
         <v>0</v>
       </c>
       <c r="K61" s="56" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -22756,25 +22969,25 @@
         <v>101020064</v>
       </c>
       <c r="B62" s="57" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="C62" s="56" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D62" s="57" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="E62" s="57" t="s">
         <v>148</v>
       </c>
       <c r="F62" s="57" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="G62" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H62" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I62" s="58">
         <v>1.5</v>
@@ -22783,7 +22996,7 @@
         <v>0</v>
       </c>
       <c r="K62" s="56" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
     </row>
     <row r="63" spans="1:11">
@@ -22791,25 +23004,25 @@
         <v>101020065</v>
       </c>
       <c r="B63" s="57" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="C63" s="56" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="D63" s="57" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="E63" s="57" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="F63" s="57" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="G63" s="57" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H63" s="57" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I63" s="58">
         <v>1.5</v>
@@ -22818,7 +23031,7 @@
         <v>0</v>
       </c>
       <c r="K63" s="56" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
     </row>
   </sheetData>
@@ -22923,10 +23136,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D4" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="E4" s="47">
         <v>50</v>
@@ -22946,7 +23159,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="D5" t="s">
         <v>107</v>
@@ -23255,8 +23468,8 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -23334,7 +23547,7 @@
         <v>Fish_Common_Shiner_Young</v>
       </c>
       <c r="B4" s="87" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="C4" s="87" t="s">
         <v>165</v>
@@ -23355,7 +23568,7 @@
         <v>Fish_Common_Shiner_Common</v>
       </c>
       <c r="B5" s="87" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="C5" s="87" t="s">
         <v>158</v>
@@ -23586,7 +23799,7 @@
         <v>Fish_Yaqui_Sucker_Young</v>
       </c>
       <c r="B16" s="87" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="C16" s="87" t="s">
         <v>165</v>
@@ -23607,7 +23820,7 @@
         <v>Fish_Yaqui_Sucker_Common</v>
       </c>
       <c r="B17" s="87" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="C17" s="87" t="s">
         <v>158</v>
@@ -23628,7 +23841,7 @@
         <v>Fish_Yaqui_Sucker_Trophy</v>
       </c>
       <c r="B18" s="87" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="C18" s="87" t="s">
         <v>159</v>
@@ -23649,7 +23862,7 @@
         <v>Fish_Yaqui_Sucker_Unique</v>
       </c>
       <c r="B19" s="87" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="C19" s="87" t="s">
         <v>160</v>
@@ -23754,7 +23967,7 @@
         <v>Fish_Bigmouth_Buffalo_Young</v>
       </c>
       <c r="B24" s="87" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="C24" s="87" t="s">
         <v>165</v>
@@ -23775,7 +23988,7 @@
         <v>Fish_Bigmouth_Buffalo_Common</v>
       </c>
       <c r="B25" s="87" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="C25" s="87" t="s">
         <v>158</v>
@@ -23796,7 +24009,7 @@
         <v>Fish_Bigmouth_Buffalo_Trophy</v>
       </c>
       <c r="B26" s="87" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="C26" s="87" t="s">
         <v>159</v>
@@ -23817,7 +24030,7 @@
         <v>Fish_Bigmouth_Buffalo_Unique</v>
       </c>
       <c r="B27" s="87" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="C27" s="87" t="s">
         <v>160</v>
@@ -24048,7 +24261,7 @@
         <v>Fish_Common_Shiner_Young</v>
       </c>
       <c r="B38" s="87" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="C38" s="87" t="s">
         <v>165</v>
@@ -24069,7 +24282,7 @@
         <v>Fish_Common_Shiner_Common</v>
       </c>
       <c r="B39" s="87" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="C39" s="87" t="s">
         <v>158</v>
@@ -24216,7 +24429,7 @@
         <v>Fish_American_Shad_Young</v>
       </c>
       <c r="B46" s="87" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="C46" s="87" t="s">
         <v>165</v>
@@ -24228,7 +24441,7 @@
         <v>15</v>
       </c>
       <c r="F46" s="35">
-        <v>52</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -24237,7 +24450,7 @@
         <v>Fish_American_Shad_Common</v>
       </c>
       <c r="B47" s="87" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="C47" s="87" t="s">
         <v>158</v>
@@ -24246,10 +24459,10 @@
         <v>2</v>
       </c>
       <c r="E47" s="35">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="F47" s="35">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -24312,7 +24525,7 @@
         <v>15</v>
       </c>
       <c r="F50" s="35">
-        <v>71</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -24330,10 +24543,10 @@
         <v>2</v>
       </c>
       <c r="E51" s="35">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="F51" s="35">
-        <v>109</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -24405,7 +24618,7 @@
         <v>Fish_Redfin_Pickerel_Young</v>
       </c>
       <c r="B55" s="87" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="C55" s="87" t="s">
         <v>165</v>
@@ -24426,7 +24639,7 @@
         <v>Fish_Redfin_Pickerel_Common</v>
       </c>
       <c r="B56" s="87" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="C56" s="87" t="s">
         <v>158</v>
@@ -24447,7 +24660,7 @@
         <v>Fish_Redfin_Pickerel_Trophy</v>
       </c>
       <c r="B57" s="87" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="C57" s="87" t="s">
         <v>159</v>
@@ -29631,7 +29844,7 @@
         <v>3</v>
       </c>
       <c r="P17" s="19" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="28.5" customHeight="1">

</xml_diff>